<commit_message>
Committing to folder structure
</commit_message>
<xml_diff>
--- a/04_API/api.xlsx
+++ b/04_API/api.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>Table 1</t>
   </si>
@@ -154,16 +154,22 @@
     <t>username: String</t>
   </si>
   <si>
-    <t>200 OK “Retrieved user userinfo”                                                         400 Bad request “Gamer not found”</t>
-  </si>
-  <si>
-    <t>/connect</t>
+    <t>200 OK “Retrieved user rinfo”                                                         400 Bad request “Gamer not found”</t>
+  </si>
+  <si>
+    <t>/connect                        /*Connection of user with other user*/</t>
   </si>
   <si>
     <t>/profile</t>
   </si>
   <si>
+    <t>200 OK “Retrieved profile”                                                                    401 Bad request “Invalid profile”</t>
+  </si>
+  <si>
     <t>/leaderboard</t>
+  </si>
+  <si>
+    <t>200 OK "Retrieved leaderboard”                              401 Bad request “Invalid profile”</t>
   </si>
 </sst>
 </file>
@@ -384,7 +390,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -431,9 +437,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1505,7 +1508,7 @@
     <col min="5" max="5" width="41" style="1" customWidth="1"/>
     <col min="6" max="6" width="33.3516" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.1719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="50.6719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.1562" style="1" customWidth="1"/>
     <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1755,36 +1758,44 @@
       <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="B13" t="s" s="16">
+      <c r="B13" t="s" s="12">
         <v>18</v>
       </c>
       <c r="C13" t="s" s="13">
         <v>41</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" t="s" s="13">
+        <v>38</v>
+      </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="H13" t="s" s="13">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" ht="56.3" customHeight="1">
       <c r="A14" s="11">
         <v>12</v>
       </c>
-      <c r="B14" t="s" s="16">
+      <c r="B14" t="s" s="12">
         <v>18</v>
       </c>
       <c r="C14" t="s" s="13">
-        <v>42</v>
-      </c>
-      <c r="D14" s="14"/>
+        <v>43</v>
+      </c>
+      <c r="D14" t="s" s="13">
+        <v>38</v>
+      </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="H14" t="s" s="13">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="15"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1794,7 +1805,7 @@
       <c r="H15" s="14"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="17"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="15"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -1804,7 +1815,7 @@
       <c r="H16" s="14"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="15"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -1814,7 +1825,7 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="15"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -1824,7 +1835,7 @@
       <c r="H18" s="14"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="17"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="15"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -1834,7 +1845,7 @@
       <c r="H19" s="14"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="15"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -1844,7 +1855,7 @@
       <c r="H20" s="14"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="17"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="15"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -1854,7 +1865,7 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="15"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -1864,7 +1875,7 @@
       <c r="H22" s="14"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="15"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
@@ -1874,7 +1885,7 @@
       <c r="H23" s="14"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="15"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -1884,7 +1895,7 @@
       <c r="H24" s="14"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="17"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="15"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -1894,7 +1905,7 @@
       <c r="H25" s="14"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="17"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="15"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>

</xml_diff>

<commit_message>
Added the check index API
</commit_message>
<xml_diff>
--- a/04_API/api.xlsx
+++ b/04_API/api.xlsx
@@ -70,7 +70,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="15"/>
+        <color indexed="16"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>max.verstappen@redbull.com</t>
@@ -204,11 +204,11 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="15"/>
+      <color indexed="16"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +233,12 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -390,7 +396,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -418,10 +424,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -430,10 +439,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -465,6 +477,7 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff4dac2b"/>
       <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
@@ -1508,7 +1521,7 @@
     <col min="5" max="5" width="41" style="1" customWidth="1"/>
     <col min="6" max="6" width="33.3516" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.1719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.1562" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.1719" style="1" customWidth="1"/>
     <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1561,358 +1574,358 @@
         <v>10</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" t="s" s="9">
+      <c r="E3" t="s" s="11">
         <v>11</v>
       </c>
-      <c r="F3" t="s" s="9">
+      <c r="F3" t="s" s="11">
         <v>12</v>
       </c>
       <c r="G3" s="10"/>
-      <c r="H3" t="s" s="9">
+      <c r="H3" t="s" s="11">
         <v>13</v>
       </c>
     </row>
     <row r="4" ht="52.9" customHeight="1">
-      <c r="A4" s="11">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="12">
+      <c r="B4" t="s" s="13">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="13">
+      <c r="C4" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" t="s" s="13">
+      <c r="D4" s="15"/>
+      <c r="E4" t="s" s="16">
         <v>15</v>
       </c>
-      <c r="F4" t="s" s="13">
+      <c r="F4" t="s" s="16">
         <v>16</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" t="s" s="13">
+      <c r="G4" s="15"/>
+      <c r="H4" t="s" s="16">
         <v>17</v>
       </c>
     </row>
     <row r="5" ht="52.9" customHeight="1">
-      <c r="A5" s="11">
+      <c r="A5" s="12">
         <v>2</v>
       </c>
-      <c r="B5" t="s" s="12">
+      <c r="B5" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="C5" t="s" s="13">
+      <c r="C5" t="s" s="16">
         <v>19</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" t="s" s="13">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" t="s" s="16">
         <v>21</v>
       </c>
     </row>
     <row r="6" ht="45.15" customHeight="1">
-      <c r="A6" s="11">
+      <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" t="s" s="12">
+      <c r="B6" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="C6" t="s" s="13">
+      <c r="C6" t="s" s="14">
         <v>23</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" t="s" s="13">
+      <c r="D6" s="15"/>
+      <c r="E6" t="s" s="16">
         <v>24</v>
       </c>
-      <c r="F6" t="s" s="13">
+      <c r="F6" t="s" s="16">
         <v>25</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" t="s" s="13">
+      <c r="G6" s="15"/>
+      <c r="H6" t="s" s="16">
         <v>26</v>
       </c>
     </row>
     <row r="7" ht="47.55" customHeight="1">
-      <c r="A7" s="11">
+      <c r="A7" s="12">
         <v>5</v>
       </c>
-      <c r="B7" t="s" s="12">
+      <c r="B7" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="C7" t="s" s="13">
+      <c r="C7" t="s" s="14">
         <v>27</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" t="s" s="13">
+      <c r="D7" s="15"/>
+      <c r="E7" t="s" s="16">
         <v>24</v>
       </c>
-      <c r="F7" t="s" s="13">
+      <c r="F7" t="s" s="16">
         <v>25</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" t="s" s="13">
+      <c r="G7" s="15"/>
+      <c r="H7" t="s" s="16">
         <v>26</v>
       </c>
     </row>
     <row r="8" ht="46.35" customHeight="1">
-      <c r="A8" s="11">
+      <c r="A8" s="12">
         <v>6</v>
       </c>
-      <c r="B8" t="s" s="12">
+      <c r="B8" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="C8" t="s" s="13">
+      <c r="C8" t="s" s="14">
         <v>28</v>
       </c>
-      <c r="D8" t="s" s="13">
+      <c r="D8" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" t="s" s="13">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" t="s" s="16">
         <v>30</v>
       </c>
     </row>
     <row r="9" ht="49.05" customHeight="1">
-      <c r="A9" s="11">
+      <c r="A9" s="12">
         <v>7</v>
       </c>
-      <c r="B9" t="s" s="12">
+      <c r="B9" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="C9" t="s" s="13">
+      <c r="C9" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="D9" t="s" s="13">
+      <c r="D9" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" t="s" s="13">
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" t="s" s="16">
         <v>32</v>
       </c>
     </row>
     <row r="10" ht="52.1" customHeight="1">
-      <c r="A10" s="11">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
-      <c r="B10" t="s" s="12">
+      <c r="B10" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="C10" t="s" s="13">
+      <c r="C10" t="s" s="16">
         <v>33</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" t="s" s="13">
+      <c r="D10" s="15"/>
+      <c r="E10" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="F10" t="s" s="13">
+      <c r="F10" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" t="s" s="13">
+      <c r="G10" s="15"/>
+      <c r="H10" t="s" s="16">
         <v>36</v>
       </c>
     </row>
     <row r="11" ht="52.1" customHeight="1">
-      <c r="A11" s="11">
+      <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" t="s" s="12">
+      <c r="B11" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="C11" t="s" s="13">
+      <c r="C11" t="s" s="16">
         <v>37</v>
       </c>
-      <c r="D11" t="s" s="13">
+      <c r="D11" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" t="s" s="13">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" t="s" s="16">
         <v>39</v>
       </c>
     </row>
     <row r="12" ht="55.5" customHeight="1">
-      <c r="A12" s="11">
+      <c r="A12" s="12">
         <v>10</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" t="s" s="13">
+      <c r="B12" s="17"/>
+      <c r="C12" t="s" s="16">
         <v>40</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" ht="50.75" customHeight="1">
-      <c r="A13" s="11">
+      <c r="A13" s="12">
         <v>11</v>
       </c>
-      <c r="B13" t="s" s="12">
+      <c r="B13" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="C13" t="s" s="13">
+      <c r="C13" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="D13" t="s" s="13">
+      <c r="D13" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" t="s" s="13">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" t="s" s="16">
         <v>42</v>
       </c>
     </row>
     <row r="14" ht="56.3" customHeight="1">
-      <c r="A14" s="11">
+      <c r="A14" s="12">
         <v>12</v>
       </c>
-      <c r="B14" t="s" s="12">
+      <c r="B14" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="C14" t="s" s="13">
+      <c r="C14" t="s" s="16">
         <v>43</v>
       </c>
-      <c r="D14" t="s" s="13">
+      <c r="D14" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" t="s" s="13">
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" t="s" s="16">
         <v>44</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="16"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="16"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="16"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="16"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="16"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="16"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="16"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="16"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>